<commit_message>
SK-10 Sortering + SK-11 Datumsformat
</commit_message>
<xml_diff>
--- a/templates/pick_up_template.xlsx
+++ b/templates/pick_up_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\Enterprise\SvenskaKyrkan\Report\Test\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F1F08F-FAB5-4180-BEBE-0078680D6BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCDE7B5-383C-4F95-98C0-32AD0AAAF2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="5" r:id="rId1"/>
@@ -91,7 +91,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_-[$€-C07]\ * #,##0.00_-;\-[$€-C07]\ * #,##0.00_-;_-[$€-C07]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -228,9 +228,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,6 +239,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,41 +528,41 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.44140625" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="19"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -579,16 +579,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20">
         <v>0</v>
       </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
         <v>1</v>
       </c>
       <c r="C6" s="5"/>
@@ -598,8 +598,8 @@
       <c r="G6" s="6"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="12"/>
@@ -607,7 +607,7 @@
       <c r="G7" s="4"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
         <v>4</v>
       </c>

</xml_diff>